<commit_message>
updated event_table for today with manual IDs
</commit_message>
<xml_diff>
--- a/data/manual assessment_combined_2024-05-23.xlsx
+++ b/data/manual assessment_combined_2024-05-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selene.Fregosi\Documents\GitHub\cross-platform-classification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5359BC70-CC62-48DA-B194-EDCC3D12BBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC27EAD-AFCE-4F8D-B6AF-EB8444A7F0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1836" yWindow="0" windowWidth="19632" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allPicks_phase3_2024-04-29" sheetId="1" r:id="rId1"/>
@@ -2256,9 +2256,9 @@
   </sheetPr>
   <dimension ref="A1:O1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K419" sqref="K419"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K399" sqref="K399:K424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2269,7 +2269,7 @@
     <col min="4" max="4" width="3.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="25" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" style="25" customWidth="1"/>
@@ -2279,7 +2279,7 @@
     <col min="15" max="15" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="36" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="36" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>

</xml_diff>